<commit_message>
Update .gitignore and joblist
</commit_message>
<xml_diff>
--- a/joblist.xlsx
+++ b/joblist.xlsx
@@ -476,42 +476,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-03-26T07:39:56Z</t>
+          <t>2025-03-23T20:15:43Z</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dotnet Developer C# Asset Management</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Apptad Inc</t>
+          <t>DUAL North America</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$249,600.00 - $270,400.00</t>
+          <t>$79,831.70 - $79,831.70</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112093137?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5108199445?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Mandatory Skills: Django, Flask, Nginx, .Net (C#) Good to Have Skills : Apache Spark Need Candidate with 10 years of relevant experience and 8 years' experience in design and develop in Asset Management Investments front office or middle office application development 5 years' experience in developing applications in Net (C#) Advocate of high code quality thru effective code reviews automation and application security Comfortable to work in a globally distributed team environment capable to lea…</t>
+          <t>At DUAL North America, our core values dictate how we live and work. We are a group with independence and people at its heart and we are a home for talent with a unique culture: the biggest small company in the world. The focus on being a People First business has always been at the very heart of the Group; Our vision was to create an independent business with a unique culture and one that would survive and thrive as a business controlled by the people working for it. And finding the most talen…</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -528,22 +528,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-03-25T07:43:14Z</t>
+          <t>2025-03-26T20:38:28Z</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Senior Android Mobile Developer</t>
+          <t>Software Developer Lead</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>VDart Inc</t>
+          <t>Tentamus North America</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Grand Prairie</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -553,17 +553,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$149,760.00 - $149,760.00</t>
+          <t>$95,000.00 - $120,000.00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014303?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5112827668?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Job Title: Senior Android Mobile Developer Location: Dallas, TX - Onsite Duration: 6 months Contract Job Description: The Senior Android Mobile Developer is responsible for end-to-end design, development and delivery for the Application Development IT initiatives including on-going enhancements and third level support of these applications. The Senior Android Mobile Developer position will contribute to the regular releases of custom mobile applications for Android platforms and supports enterp…</t>
+          <t>DO YOU EXCEL AT LEADING TECHNICAL PROJECTS AND DRIVING INNOVATIVE SOFTWARE SOLUTIONS? Tentamus North America is on the prowl for a Technical Project Manager to spearhead IT ini tiatives , optimize software configurations, and collaborate with cross-functional teams to enhance laboratory operations. This role is perfect for someone with a strong technical background, exceptional project management skills, and the ability to bridge the gap between software solutions and business needs. If you thr…</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -580,42 +580,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-03-25T07:43:11Z</t>
+          <t>2025-03-25T01:25:15Z</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Senior Android Mobile Developer</t>
+          <t>Bilingual Software Developer</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Inherent Technologies</t>
+          <t>Cinter Career</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Addison</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$93,381.14 - $93,381.14</t>
+          <t>$89,682.83 - $89,682.83</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014241?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5109637170?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Must have skill: C#, Android mobile development, Xamarin, Kotlin, .NET MAUI, Terraform, Azure Dev-ops Job Summary: The Senior Android Mobile Developer is responsible for end-to-end design, development and delivery for the Application Development IT initiatives including on-going enhancements and third level support of these applications. The Senior Android Mobile Developer position will contribute to the regular releases of custom mobile applications for Android platforms and supports enterpris…</t>
+          <t>Job Description Job Description Client (type/ industry): Software Engineering Company Working Location: Dallas, TX Employment Type: Full-time (40hours/week) Language: Japanese and English Salary: 80K – 100K (DOE) Job Overview Responsible for overseeing, participating in, and performing (but not limited to) the following tasks: Design and develop software for embedded systems Implement FPGA designs Develop applications using programming languages such as Flutter, Java, and C Test and debug softw…</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -632,42 +632,42 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-03-25T07:43:12Z</t>
+          <t>2025-03-24T19:09:20Z</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Apptad - Senior Android Mobile Developer</t>
+          <t>Senior Backend Software Developer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Apptad Inc</t>
+          <t>Gravitate</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$124,800.00 - $135,200.00</t>
+          <t>$97,983.99 - $97,983.99</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014273?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5109416967?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Job Title: Senior Android Mobile Developer Location: Dallas, TX (Onsite from day 1, need only local profiles) Duration: 6 Months contract with possible extension Must have Skills: C#, Android mobile development, Xamarin, .NET MAUI, Terraform, Azure Dev-ops Job Summary: The Senior Android Mobile Developer is responsible for end-to-end design, development and delivery for the Application Development IT initiatives including on-going enhancements and third level support of these applications. The …</t>
+          <t>Why Gravitate? At Gravitate, we’re on a mission to put everyday supply and logistics decisions in motion, powered by innovative problem-solving from industry experts. A lot of companies say it. We mean it: Gravitate is different. Rooted in the spirit of collaboration, we thrive on the smarts of our people and the dynamic we’ve cultivated. What will you be doing? You will work within capSpire's flagship software product, Gravitate. Gravitate provides AI-enabled collaboration, automation, and dec…</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -684,22 +684,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-03-25T07:43:47Z</t>
+          <t>2025-03-24T17:49:30Z</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Senior Android Mobile Developer</t>
+          <t>Associate Director, Software Development</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Noblesoft Technologies</t>
+          <t>Verizon</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -709,69 +709,67 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$135,200.00 - $149,760.00</t>
+          <t>$232,465.44 - $232,465.44</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014924?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5109365182?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Update on 03/24: New role, need local profiles Job Title: Senior Android Mobile Developer Location: Dallas, TX (Onsite from day 1, need only local profiles) Duration: 6 Months Must have skill: C#, Android mobile development, Xamarin, .NET MAUI, Terraform, Azure Dev-ops Job Summary: The Senior Android Mobile Developer is responsible for end-to-end design, development and delivery for the Application Development IT initiatives including on-going enhancements and third level support of these appli…</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+          <t>When you join Verizon You want more out of a career. A place to share your ideas freely - even if they're daring or different. Where the true you can learn, grow, and thrive. At Verizon, we power and empower how people live, work and play by connecting them to what brings them joy. We do what we love - driving innovation, creativity, and impact in the world. Our V Team is a community of people who anticipate, lead, and believe that listening is where learning begins. In crisis and in celebratio…</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>3.3</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>2420 N Belt Line Rd,Ste 150,Irving, TX 75062</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-03-23T07:08:37Z</t>
+          <t>2025-03-26T01:41:29Z</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Java &amp; Angular Web Developer Job at Mindlance in Irving</t>
+          <t>Senior Front End Software Developer</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Mindlance</t>
+          <t>VYNYL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$75,190.01 - $75,190.01</t>
+          <t>$80,727.45 - $80,727.45</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5107606131?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5111771594?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>JOB DESCRIPTION: Angular Web Developer Duration: 1 Year (possible extension or conversion) Location: ONSITE REQUIREMENT - 2/3 days per week IRVING , TX 75039 Will interview in the mornings up to 2 per day. times are consistent at 9am and 10am Angular Web Developer Client is seeking an Angular Web Developer to work on creating a web-based UI for Account Master Central platform. The platform consists of sophisticated Line of Business functions presented using hundreds of screens. The role involve…</t>
+          <t>Job Description Job Description Vynyl delivers high-fidelity software and design to leading companies in finance, health, and other industries. We solve important and valuable problems in the areas of Product Design &amp; Development, Cloud Operations and Cloud Migration, Security, Business Intelligence, and Health Data Interoperability. We engage with clients using our Scrum-based agile methodology and we like nothing more than the opportunity to demo the latest iteration of the software or design…</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -788,22 +786,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-03-23T07:07:52Z</t>
+          <t>2025-03-27T14:32:15Z</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mindlance is hiring: Java &amp; Angular Web Developer in Irving</t>
+          <t>Field Service Technician</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Mindlance</t>
+          <t>Lincoln Electric</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Coppell</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -813,17 +811,17 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$80,311.40 - $80,311.40</t>
+          <t>$55,176.01 - $55,176.01</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5107599018?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/land/ad/5113969747?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=0CE363695D8A4BC65D1E680BDCDB34F6DE138A04</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>JOB DESCRIPTION: Angular Web Developer Duration: 1 Year (possible extension or conversion) Location: ONSITE REQUIREMENT - 2/3 days per week IRVING , TX 75039 Will interview in the mornings up to 2 per day. times are consistent at 9am and 10am Angular Web Developer Client is seeking an Angular Web Developer to work on creating a web-based UI for Account Master Central platform. The platform consists of sophisticated Line of Business functions presented using hundreds of screens. The role involve…</t>
+          <t>Lincoln Electric is the world leader in the engineering, design, and manufacturing of advanced arc welding solutions, automated joining, assembly and cutting systems, plasma and oxy-fuel cutting equipment, and has a leading global position in brazing and soldering alloys. Lincoln is recognized as the Welding Expert™ for its leading materials science, software development, automation engineering, and application expertise, which advance customers' fabrication capabilities to help them build a be…</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -840,22 +838,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-03-26T15:23:17Z</t>
+          <t>2025-03-25T12:43:17Z</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Angular Web Developer</t>
+          <t>Platform - Engineering Productivity - Software Engineer</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Axelon</t>
+          <t>Elastic</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Highland Park</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -865,17 +863,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$71,980.10 - $71,980.10</t>
+          <t>$135,434.08 - $135,434.08</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112647103?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110640622?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Global Financial Firm located in Irving, TX has an immediate contract opportunity for an experienced ngular Web Developer "This role is currently on a Hybrid Schedule. You will need to have reliable internet, computer and android or iphone for remote access into the client systems during remote work. We will be expected in the office weekly 3 days depending on the team requirement. Video/ f2f interviews are required prior to all offers. Job Description: ngular Web Developer Information Services…</t>
+          <t>Elastic, the Search AI Company, enables everyone to find the answers they need in real time, using all their data, at scale — unleashing the potential of businesses and people. The Elastic Search AI Platform, used by more than 50% of the Fortune 500, brings together the precision of search and the intelligence of AI to enable everyone to accelerate the results that matter. By taking advantage of all structured and unstructured data — securing and protecting private information more effectively …</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -892,22 +890,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-03-26T07:40:06Z</t>
+          <t>2025-03-25T12:43:12Z</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Senior AWS Developer</t>
+          <t>Business Systems Analyst, HR Systems</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Excelon Solutions</t>
+          <t>Elastic</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Coppell</t>
+          <t>Highland Park</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -917,17 +915,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$111,337.27 - $111,337.27</t>
+          <t>$80,081.12 - $80,081.12</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112093787?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110640535?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Client: BRINKS Job title: Senior AWS Developer Location: Onsite at Coppell, TX Duration: 9 months Visa: USC / GC / EADs Rate: $ 55-57 /hr W-2 Interview: 3 Round Process (2nd Round is On-Site Technical Coding) Years of Experience : 5 Professional YOE MUST HAVES: AWS Cloud Experience, C#, Terraform, Lambda, SNS Quere, S3, CI/CD, Serverless Function Experience NICE TO HAVE: Azure Exposure, UI Experience, Experience working with Delivery/Logistics Company Target Companies/ Previous clients: UPS, Fe…</t>
+          <t>Elastic, the Search AI Company, enables everyone to find the answers they need in real time, using all their data, at scale — unleashing the potential of businesses and people. The Elastic Search AI Platform, used by more than 50% of the Fortune 500, brings together the precision of search and the intelligence of AI to enable everyone to accelerate the results that matter. By taking advantage of all structured and unstructured data — securing and protecting private information more effectively …</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -944,42 +942,42 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-03-27T07:36:37Z</t>
+          <t>2025-03-23T01:05:25Z</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Healthcare Integration Specialist</t>
+          <t>Junior IT Project Manager - REMOTE WORK - 62818</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>VDart Inc</t>
+          <t>PRIMUS Global Services, Inc</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$145,600.00 - $166,400.00</t>
+          <t>$95,274.60 - $95,274.60</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5113399140?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/land/ad/5107279675?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=C674E4EFC8BAF8F41DBDADEC791FD7EE266BA462</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Healthcare Integration Specialist Dallas, TX (Hybrid/Remote) Contract We are seeking a Healthcare Platform Integration Specialist to lead the integration of Healthcare Platform with Electronic Medical Records (EMR) systems. This role involves designing, implementing, and maintaining seamless data exchange workflows while ensuring regulatory compliance and system interoperability. The ideal candidate will have a strong background in healthcare IT, system integration, HL7 FHIR standards, and EMR …</t>
+          <t>Job Description Job Description Junior IT Project Manager - 62818 We have an immediate long-term opportunity with one of our prime clients for the position of Junior IT Project Manager to work on Remote basis. Pay Rate : $30-$35/hr Interview Process: Initial interview with the hiring manager and other PMO Managers Second round interview with PMO Director Must Have:- Any 2-5 years IT PM who has worked on SDLC-related projects and is in Texas should work as long as communication is great. Ideal C…</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -996,17 +994,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-03-25T19:40:10Z</t>
+          <t>2025-03-27T16:16:04Z</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>C++ Software Engineer</t>
+          <t>▷ [Apply Now] Travel Cardiac Cath Lab RN</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Davanti</t>
+          <t>Genie Healthcare</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1021,17 +1019,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>$102,288.94 - $102,288.94</t>
+          <t>$107,299.55 - $107,299.55</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5111388677?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/land/ad/5114560880?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=C4BE83887125FC631790DA8D0BC686D9503922A5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Do you want to tackle the biggest questions in finance with near infinite compute power at your fingertips? G-Research is a leading quantitative research and technology firm, with offices in London and Dallas. We are proud to employ some of the best people in their field and to nurture their talent in a dynamic, flexible and highly stimulating culture where world-beating ideas are cultivated and rewarded. This is a hybrid role based in our new Dallas infrastructure hub where we work on the late…</t>
+          <t>Job Description Genie Healthcare is seeking a travel nurse RN Cardiac Cath Lab for a travel nursing job in Dallas, Texas. Job Description &amp; Requirements - Specialty: Cardiac Cath Lab - Discipline: RN - Start Date: ASAP - Duration: 13 weeks - 40 hours per week - Shift: 10 hours, days - Employment Type: Travel Genie Healthcare is looking for a Cardiology to work in Cath Lab Tech for a 13 weeks travel assignment located in Dallas, TX for the Shift (4x10 Days-Please verify shift details with recrui…</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1048,22 +1046,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-03-27T07:07:04Z</t>
+          <t>2025-03-26T13:33:43Z</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Lead Software Engineer</t>
+          <t>Senior Java Software Engineer (Onsite)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Wells Fargo</t>
+          <t>Raytheon</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Richardson</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1073,44 +1071,42 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>$145,262.98 - $145,262.98</t>
+          <t>$127,169.59 - $127,169.59</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5113368975?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/land/ad/5112312453?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=37623A25694F1B4BB713B319DD0104C8376F6931</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>About this role: In this role, you will act as a .NET Engineer for an agile team providing application design, testing, implementation support, and execution; utilizing a thorough understanding of applicable technology with an underlying migration goal to cloud based technologies. You will be responsible for analyzing complex business requirements and designs specifications, converting them into user stories and tasks and completing the tasks within allocated sprints. This engineer will need an…</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+          <t>Date Posted: 2025-02-26 Country: United States of America Location: TX233: Richardson 1737 CityLine 1737 East CityLine Drive Building C37, Richardson, TX, 75082 USA Position Role Type: Onsite At Raytheon, the foundation of everything we do is rooted in our values and a higher calling – to help our nation and allies defend freedoms and deter aggression. We bring the strength of more than 100 years of experience and renowned engineering expertise to meet the needs of today’s mission and stay ahea…</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>2501 W University Dr,McKinney, TX 75071</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-03-24T01:21:54Z</t>
+          <t>2025-03-24T20:49:00Z</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Senior LabVIEW Engineer</t>
+          <t>Principal Software Engineer</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CyberCoders</t>
+          <t>The Expo Group</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1125,17 +1121,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>$110,000.00 - $150,000.00</t>
+          <t>$120,384.30 - $120,384.30</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5108365563?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5109470934?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Senior LabVIEW Engineer For the past 30 years we've been making an impact in the aerospace, defense and energy industries - specifically centered around creating reliable test and measurement solutions. Our team has many awards under our belt that stem from our design and build structure of our test systems. Our footprint extends into Electrical, Mechanical, RF Test Systems and were recently listed as one of the fastest growing small businesses in the country. What You Will Be Doing - Project r…</t>
+          <t>Join Our Innovative Team as a Principal Software Engineer Are you ready to drive software innovation and collaborate with a dynamic team? The Expo Group is seeking a Principal Software Engineer to design, develop, and optimize software applications that meet the needs of a growing, innovative company. Based in Irving or remotely, this role will be crucial in enhancing our software solutions while working closely with cross-functional teams to deliver scalable and efficient systems. In this role…</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1152,42 +1148,42 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-03-26T01:40:33Z</t>
+          <t>2025-03-25T07:43:28Z</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sr .NET Full Stack Developer</t>
+          <t>C++ Developer (Audio/Video)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Resource Informatics Group Inc</t>
+          <t>TalentOla</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Highland Park</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>$80,649.65 - $80,649.65</t>
+          <t>$100,612.38 - $100,612.38</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5111766266?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110014569?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Job Description Job Description Role : Sr .NET Full Stack Developer Location : Dallas, TX (Remote till covid) Duration : 06 Months Plus Visa : Independent Consultants Only (As per EC requirement) End Client : Confidential till resume selection Rate : $52 on CTC. Description: · Experience troubleshooting &amp; refactoring existing web applications · Experience migrating applications to a new host (migration to Azure Cloud is highly preferred) · Experience with YAML or JSON – building pipelines · Exp…</t>
+          <t>Title: C++ Developer (Audio/Video) Location: Dallas, TX (5 day onsite) Job Description 8 years of relevant software development experience Extensive experience in C/C++ development, including a solid understanding of audio/video technologies with a commitment to delivering high-quality software through adherence to coding standards and testing practices. Must Have: Experience in C/C++, Strong in Linux system programming , good understanding what ABI is, library dependencies, cross-compilation. …</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1204,42 +1200,42 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-03-26T20:38:28Z</t>
+          <t>2025-03-23T23:20:54Z</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Software Developer Lead</t>
+          <t>Senior/Staff Software Engineer - Front End Platform</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Tentamus North America</t>
+          <t>Polly</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Grand Prairie</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$95,000.00 - $120,000.00</t>
+          <t>$170,339.92 - $170,339.92</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112827668?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5108299538?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>DO YOU EXCEL AT LEADING TECHNICAL PROJECTS AND DRIVING INNOVATIVE SOFTWARE SOLUTIONS? Tentamus North America is on the prowl for a Technical Project Manager to spearhead IT ini tiatives , optimize software configurations, and collaborate with cross-functional teams to enhance laboratory operations. This role is perfect for someone with a strong technical background, exceptional project management skills, and the ability to bridge the gap between software solutions and business needs. If you thr…</t>
+          <t>Who You Are: You have 6 years of software development experience under your belt and are looking for your next challenge in a hyper-growth, fast-paced, industry disrupting, SaaS company. You are excited to work with emerging technologies and modern tech stack with a collaborative engineering team, where you will have a direct impact in the delivery of first class software products. Your experience mentoring others, working with distributed systems, relational databases, and all things software …</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1256,22 +1252,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-03-26T22:15:26Z</t>
+          <t>2025-03-25T07:43:28Z</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Senior Fullstack Engineer</t>
+          <t>C++ Embedded Engineer</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wellfit Technologies</t>
+          <t>TalentOla</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Cockrell Hill</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1281,17 +1277,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$172,693.34 - $172,693.34</t>
+          <t>$94,271.09 - $94,271.09</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112872271?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110014562?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Wellfit is the dental industry’s fintech solution A healthcare fintech company that enhances experiences between patients, providers, employers and payors. Wellfit provides access to treatment and care of all by removing financial barriers. About the Role The Sr. Software Engineer position, is a key role for our organization. You will be immersed in a high performing and frequently challenged team responsible for multiple software products developed by Wellfit. You will lead and/or consult with…</t>
+          <t>Title: C++ Embedded Engineer Location: Dallas, TX (Onsite in office) Job Description: Experience in architecture, design, prototyping, software development, code review and unit testing for embedded devices. Experience with modern C, C++, C++11/C++14 or C++17 preferred. Experience in Embedded systems. Experience in C, C++ , embedded Linux and device driver Experience with POSIX-based embedded systems, one or more of Linux, QNX. Experience with Linux, BSP, Linux subsystems Memory and performance…</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1308,42 +1304,42 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-03-24T20:49:00Z</t>
+          <t>2025-03-26T19:25:33Z</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Principal Software Engineer</t>
+          <t>Technical Project Manager</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>The Expo Group</t>
+          <t>Axiom Software Solutions Limited</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$120,384.30 - $120,384.30</t>
+          <t>$110,341.02 - $110,341.02</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5109470934?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5112781667?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Join Our Innovative Team as a Principal Software Engineer Are you ready to drive software innovation and collaborate with a dynamic team? The Expo Group is seeking a Principal Software Engineer to design, develop, and optimize software applications that meet the needs of a growing, innovative company. Based in Irving or remotely, this role will be crucial in enhancing our software solutions while working closely with cross-functional teams to deliver scalable and efficient systems. In this role…</t>
+          <t>Role: Technical Project Manager - Remote US Technical Project Manager with AWS, GCP experience JOB DESCRIPTION "5 years of technical program management experience in cloud infrastructure Proven track record of managing large-scale complex projects Strong technical skills and understanding of cloud computing, serverless architecture, and core infrastructure components Hands-on experience with cloud providers such as AWS, Azure, or GCP Experience in networking engineering, networking infrastructu…</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1360,42 +1356,42 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-03-23T12:10:09Z</t>
+          <t>2025-03-25T07:43:28Z</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sharepoint Developer</t>
+          <t>Senior Software Engineer (BLE, C++)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Strategic Resource Partners, Inc.</t>
+          <t>TalentOla</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Cockrell Hill</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>$82,243.61 - $82,243.61</t>
+          <t>$89,213.06 - $89,213.06</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5107868098?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110014567?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Job Description Job Description The SharePoint Specialist will be working in an organization where collaboration, together with best practice document, data and knowledge management are key elements of its operations and SharePoint is a key technology being used to address these needs. The candidate will have demonstrated extensive experience and expertise in all aspects of the duties and key responsibilities and working within a small team will be essential for the role to make a strong, hands…</t>
+          <t>Title: Senior Software Engineer (BLE, C++) Location: Dallas, TX (5 day onsite) Job Responsibilities Architect, develop and supervise the Linux based TV OS Bluetooth software Develop applications for smart TV Bluetooth audio and peripherals Port classic audio features of TV to LE Audio New application features using LE Audio Sustenance engineering of existing Bluetooth functionality on TV: Improvements, bug-fixes and new features Job Description 8 years of experience with C/C++, Linux/Unix and B…</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1412,42 +1408,42 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-03-26T20:43:30Z</t>
+          <t>2025-03-26T07:40:05Z</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Engineering - Dallas - Associate - Developer and Data Engineer</t>
+          <t>Java Full stack Developer</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Asset &amp; Wealth Management</t>
+          <t>Sumeru Solutions</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Cockrell Hill</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>$158,186.64 - $158,186.64</t>
+          <t>$122,468.09 - $122,468.09</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112834069?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5112093702?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Description The Workforce Identities Engineering team within the Identity and Access Management function of Core Engineering is looking for an experienced developer with data engineering experience. This position will be working with a global team responsible for the architecture, design and development of systems supporting the on-premise Active Directory and cloud-based identity platforms for Goldman Sachs. We are looking for developers who understand the requirements for global, distributed …</t>
+          <t>Role : Java Developer Location : Dallas, TX Must Have Skills 6 years of full Software Development Life Cycle SDLC experience designing developing and implementing largescale applications in hosted production environments 2 years Microservice framework REST development Preferred Qualifications Education Prior Job Experience 2 years of Kubernetes Services with deep understanding of Container Orchestration and Distributed System Concepts Skills Licenses Certifications Proficiency in Full Stack Dev…</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1464,42 +1460,42 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-03-26T00:07:32Z</t>
+          <t>2025-03-25T07:43:46Z</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Junior Mobile Developer</t>
+          <t>Software Engineer- Location: Addison, TX-onsite work only – Fulltime - Aerospace domain</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tech Consulting</t>
+          <t>Marvel Infotech</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Addison</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>$62,291.68 - $62,291.68</t>
+          <t>$120,000.00 - $140,000.00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5111630051?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110014904?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Job Description Job Description Job Title: Jr. Mobile Developer (Urgent hiring) Location: Dallas, TX Employment type: Fulltime Duration: 2 years Exp: 1-4 years(Entry level) Educational Qualification: Bachelor’s/Master’s Degree in Computer Science, Information Systems, Electrical Engineering, Mathematics, or a related quantitative field. Are you excited about taking your technical career to new heights with a full-time, W-2 role as a consultant in a dynamic and rapidly growing company? If you ar…</t>
+          <t>Software Engineer- Location: Addison, TX-onsite work only Fulltime - Aerospace domain Client needs 10 years of experience only Software Engineer This is an onsite, full-time position as part of our Engineering Team within the Software Development Group. The position is to design and implement properly documented, reliable software that ensures safe and proper execution of microprocessor and/or GUI based products/systems. Job Responsibilities Software design and development of microprocessor and…</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">

</xml_diff>

<commit_message>
Added .env for 'keys'
</commit_message>
<xml_diff>
--- a/joblist.xlsx
+++ b/joblist.xlsx
@@ -632,17 +632,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-03-24T19:09:20Z</t>
+          <t>2025-03-28T00:03:45Z</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Senior Backend Software Developer</t>
+          <t>Associate, Software Developer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Gravitate</t>
+          <t>Lido Advisors</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -657,17 +657,17 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$97,983.99 - $97,983.99</t>
+          <t>$69,612.12 - $69,612.12</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5109416967?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5114941185?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Why Gravitate? At Gravitate, we’re on a mission to put everyday supply and logistics decisions in motion, powered by innovative problem-solving from industry experts. A lot of companies say it. We mean it: Gravitate is different. Rooted in the spirit of collaboration, we thrive on the smarts of our people and the dynamic we’ve cultivated. What will you be doing? You will work within capSpire's flagship software product, Gravitate. Gravitate provides AI-enabled collaboration, automation, and dec…</t>
+          <t>The Investment Management team at Lido Advisors, LLC handles various cross functional domains including portfolio management, risk assessment, market research and trading. Over time the scope of responsibilities within the team has grown significantly leading to the development of proprietary technology and applications aimed at supporting the firm’s rapid growth. As a Software Developer, you will primarily be tasked with supporting existing applications along with assisting with the developmen…</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -684,144 +684,144 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-03-24T17:49:30Z</t>
+          <t>2025-03-24T19:09:20Z</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Associate Director, Software Development</t>
+          <t>Senior Backend Software Developer</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Verizon</t>
+          <t>Gravitate</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$232,465.44 - $232,465.44</t>
+          <t>$97,983.99 - $97,983.99</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5109365182?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5109416967?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>When you join Verizon You want more out of a career. A place to share your ideas freely - even if they're daring or different. Where the true you can learn, grow, and thrive. At Verizon, we power and empower how people live, work and play by connecting them to what brings them joy. We do what we love - driving innovation, creativity, and impact in the world. Our V Team is a community of people who anticipate, lead, and believe that listening is where learning begins. In crisis and in celebratio…</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>3.3</v>
+          <t>Why Gravitate? At Gravitate, we’re on a mission to put everyday supply and logistics decisions in motion, powered by innovative problem-solving from industry experts. A lot of companies say it. We mean it: Gravitate is different. Rooted in the spirit of collaboration, we thrive on the smarts of our people and the dynamic we’ve cultivated. What will you be doing? You will work within capSpire's flagship software product, Gravitate. Gravitate provides AI-enabled collaboration, automation, and dec…</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2420 N Belt Line Rd,Ste 150,Irving, TX 75062</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-03-26T01:41:29Z</t>
+          <t>2025-03-24T17:49:30Z</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Senior Front End Software Developer</t>
+          <t>Associate Director, Software Development</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>VYNYL</t>
+          <t>Verizon</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$80,727.45 - $80,727.45</t>
+          <t>$232,465.44 - $232,465.44</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5111771594?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5109365182?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Job Description Job Description Vynyl delivers high-fidelity software and design to leading companies in finance, health, and other industries. We solve important and valuable problems in the areas of Product Design &amp; Development, Cloud Operations and Cloud Migration, Security, Business Intelligence, and Health Data Interoperability. We engage with clients using our Scrum-based agile methodology and we like nothing more than the opportunity to demo the latest iteration of the software or design…</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+          <t>When you join Verizon You want more out of a career. A place to share your ideas freely - even if they're daring or different. Where the true you can learn, grow, and thrive. At Verizon, we power and empower how people live, work and play by connecting them to what brings them joy. We do what we love - driving innovation, creativity, and impact in the world. Our V Team is a community of people who anticipate, lead, and believe that listening is where learning begins. In crisis and in celebratio…</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>3.3</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>2420 N Belt Line Rd,Ste 150,Irving, TX 75062</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-03-27T14:32:15Z</t>
+          <t>2025-03-26T01:41:29Z</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Field Service Technician</t>
+          <t>Senior Front End Software Developer</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lincoln Electric</t>
+          <t>VYNYL</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Coppell</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$55,176.01 - $55,176.01</t>
+          <t>$80,727.45 - $80,727.45</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/land/ad/5113969747?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=0CE363695D8A4BC65D1E680BDCDB34F6DE138A04</t>
+          <t>https://www.adzuna.com/details/5111771594?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Lincoln Electric is the world leader in the engineering, design, and manufacturing of advanced arc welding solutions, automated joining, assembly and cutting systems, plasma and oxy-fuel cutting equipment, and has a leading global position in brazing and soldering alloys. Lincoln is recognized as the Welding Expert™ for its leading materials science, software development, automation engineering, and application expertise, which advance customers' fabrication capabilities to help them build a be…</t>
+          <t>Job Description Job Description Vynyl delivers high-fidelity software and design to leading companies in finance, health, and other industries. We solve important and valuable problems in the areas of Product Design &amp; Development, Cloud Operations and Cloud Migration, Security, Business Intelligence, and Health Data Interoperability. We engage with clients using our Scrum-based agile methodology and we like nothing more than the opportunity to demo the latest iteration of the software or design…</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -838,42 +838,42 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-03-25T12:43:17Z</t>
+          <t>2025-03-28T00:55:10Z</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Platform - Engineering Productivity - Software Engineer</t>
+          <t>Investment Banking, Software Developer, Associate, Dallas</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Elastic</t>
+          <t>Asset &amp; Wealth Management</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Highland Park</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$135,434.08 - $135,434.08</t>
+          <t>$150,675.95 - $150,675.95</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110640622?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5115218741?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Elastic, the Search AI Company, enables everyone to find the answers they need in real time, using all their data, at scale — unleashing the potential of businesses and people. The Elastic Search AI Platform, used by more than 50% of the Fortune 500, brings together the precision of search and the intelligence of AI to enable everyone to accelerate the results that matter. By taking advantage of all structured and unstructured data — securing and protecting private information more effectively …</t>
+          <t>Description INVESTMENT BANKING Goldman Sachs Investment Banking (IB) works on some of the most complex financial challenges and transactions in the market today. Whether advising on a merger, providing financial solutions for an acquisition, or structuring an initial public offering, we handle projects that help clients at major milestones. We work with corporations, pension funds, financial sponsors, and governments and are team of strong analytical thinkers, who have a passion for producing o…</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -890,22 +890,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-03-25T12:43:12Z</t>
+          <t>2025-03-27T14:32:15Z</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Business Systems Analyst, HR Systems</t>
+          <t>Field Service Technician</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Elastic</t>
+          <t>Lincoln Electric</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Highland Park</t>
+          <t>Coppell</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -915,17 +915,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$80,081.12 - $80,081.12</t>
+          <t>$55,176.01 - $55,176.01</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110640535?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/land/ad/5113969747?se=GvcZky8M8BGCrnsET3cHCQ&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=0CE363695D8A4BC65D1E680BDCDB34F6DE138A04</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Elastic, the Search AI Company, enables everyone to find the answers they need in real time, using all their data, at scale — unleashing the potential of businesses and people. The Elastic Search AI Platform, used by more than 50% of the Fortune 500, brings together the precision of search and the intelligence of AI to enable everyone to accelerate the results that matter. By taking advantage of all structured and unstructured data — securing and protecting private information more effectively …</t>
+          <t>Lincoln Electric is the world leader in the engineering, design, and manufacturing of advanced arc welding solutions, automated joining, assembly and cutting systems, plasma and oxy-fuel cutting equipment, and has a leading global position in brazing and soldering alloys. Lincoln is recognized as the Welding Expert™ for its leading materials science, software development, automation engineering, and application expertise, which advance customers' fabrication capabilities to help them build a be…</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -942,42 +942,42 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-03-23T01:05:25Z</t>
+          <t>2025-03-28T08:10:44Z</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Junior IT Project Manager - REMOTE WORK - 62818</t>
+          <t>Senior Software Engineer- .Net Developer</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PRIMUS Global Services, Inc</t>
+          <t>Schneider Electric</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Highland Park</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$95,274.60 - $95,274.60</t>
+          <t>$103,766.07 - $103,766.07</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/land/ad/5107279675?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=C674E4EFC8BAF8F41DBDADEC791FD7EE266BA462</t>
+          <t>https://www.adzuna.com/details/5115592077?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Job Description Job Description Junior IT Project Manager - 62818 We have an immediate long-term opportunity with one of our prime clients for the position of Junior IT Project Manager to work on Remote basis. Pay Rate : $30-$35/hr Interview Process: Initial interview with the hiring manager and other PMO Managers Second round interview with PMO Director Must Have:- Any 2-5 years IT PM who has worked on SDLC-related projects and is in Texas should work as long as communication is great. Ideal C…</t>
+          <t>For this U.S. based position, the expected compensation range is $ 96,000 - $144,000 per year, which includes base pay and short-term incentive. The compensation range for this full-time position applies to candidates located within the United States. Our salary ranges are determined by reviewing roles of similar responsibility and level. Within the salary range, individual pay is determined by several factors including performance, knowledge, job-related skills, experience, and relevant educat…</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -994,12 +994,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-03-27T16:16:04Z</t>
+          <t>2025-03-27T22:56:11Z</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>▷ [Apply Now] Travel Cardiac Cath Lab RN</t>
+          <t>Travel Nurse RN - Cardiac Cath Lab - $3,088 per week</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1009,27 +1009,27 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Mesquite</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>$107,299.55 - $107,299.55</t>
+          <t>Up to $160,576.00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/land/ad/5114560880?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=C4BE83887125FC631790DA8D0BC686D9503922A5</t>
+          <t>https://www.adzuna.com/land/ad/5114785311?se=GvcZky8M8BGCrnsET3cHCQ&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=3A737B1196F843E477A5B3BEFF5464424713852D</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Job Description Genie Healthcare is seeking a travel nurse RN Cardiac Cath Lab for a travel nursing job in Dallas, Texas. Job Description &amp; Requirements - Specialty: Cardiac Cath Lab - Discipline: RN - Start Date: ASAP - Duration: 13 weeks - 40 hours per week - Shift: 10 hours, days - Employment Type: Travel Genie Healthcare is looking for a Cardiology to work in Cath Lab Tech for a 13 weeks travel assignment located in Dallas, TX for the Shift (4x10 Days-Please verify shift details with recrui…</t>
+          <t>Genie Healthcare is seeking a travel nurse RN Cardiac Cath Lab for a travel nursing job in Mesquite, Texas. Job Description &amp; Requirements Specialty: Cardiac Cath Lab Discipline: RN Start Date: ASAP Duration: 13 weeks 40 hours per week Shift: 8 hours, days Employment Type: Travel Genie Healthcare is looking for a RN to work in Cath Lab for a 13 weeks travel assignment located in Mesquite, TX for the Shift (5x8 Days - Please verify shift details with recruiter, 07:00:00-15:00:00, 8.00-5). Pay an…</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1046,22 +1046,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-03-26T13:33:43Z</t>
+          <t>2025-03-28T15:45:23Z</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Senior Java Software Engineer (Onsite)</t>
+          <t>Information Services Developer Senior - IM Application Development</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Raytheon</t>
+          <t>CHRISTUS Health</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Richardson</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1071,47 +1071,47 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>$127,169.59 - $127,169.59</t>
+          <t>$74,792.23 - $74,792.23</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/land/ad/5112312453?se=quJ_CHUL8BGYKDhUAbaCew&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=37623A25694F1B4BB713B319DD0104C8376F6931</t>
+          <t>https://www.adzuna.com/land/ad/5116539275?se=GvcZky8M8BGCrnsET3cHCQ&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=E6D77BAAFD5D0E05AD84DB1D5CEF9A4786FFA0E4</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Date Posted: 2025-02-26 Country: United States of America Location: TX233: Richardson 1737 CityLine 1737 East CityLine Drive Building C37, Richardson, TX, 75082 USA Position Role Type: Onsite At Raytheon, the foundation of everything we do is rooted in our values and a higher calling – to help our nation and allies defend freedoms and deter aggression. We bring the strength of more than 100 years of experience and renowned engineering expertise to meet the needs of today’s mission and stay ahea…</t>
+          <t>Description Summary: The Information Services Developer Senior is primarily responsible for designing, developing, and implementing systems based on requirements. The candidate should have good knowledge of development methodologies and follow them while designing and coding. This role requires collaborating and working with another team member focusing on quality support to both internal and external users, focusing on customer services and timeliness. Responsibilities: Analyze ideas and busin…</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2501 W University Dr,McKinney, TX 75071</t>
+          <t>919 Hidden Ridge,Irving, TX 75038</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-03-24T20:49:00Z</t>
+          <t>2025-03-25T12:43:17Z</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Principal Software Engineer</t>
+          <t>Platform - Engineering Productivity - Software Engineer</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The Expo Group</t>
+          <t>Elastic</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Highland Park</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1121,17 +1121,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>$120,384.30 - $120,384.30</t>
+          <t>$135,434.08 - $135,434.08</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5109470934?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110640622?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Join Our Innovative Team as a Principal Software Engineer Are you ready to drive software innovation and collaborate with a dynamic team? The Expo Group is seeking a Principal Software Engineer to design, develop, and optimize software applications that meet the needs of a growing, innovative company. Based in Irving or remotely, this role will be crucial in enhancing our software solutions while working closely with cross-functional teams to deliver scalable and efficient systems. In this role…</t>
+          <t>Elastic, the Search AI Company, enables everyone to find the answers they need in real time, using all their data, at scale — unleashing the potential of businesses and people. The Elastic Search AI Platform, used by more than 50% of the Fortune 500, brings together the precision of search and the intelligence of AI to enable everyone to accelerate the results that matter. By taking advantage of all structured and unstructured data — securing and protecting private information more effectively …</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1148,17 +1148,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-03-25T07:43:28Z</t>
+          <t>2025-03-25T12:43:12Z</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>C++ Developer (Audio/Video)</t>
+          <t>Business Systems Analyst, HR Systems</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TalentOla</t>
+          <t>Elastic</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1173,17 +1173,17 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>$100,612.38 - $100,612.38</t>
+          <t>$80,081.12 - $80,081.12</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014569?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110640535?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Title: C++ Developer (Audio/Video) Location: Dallas, TX (5 day onsite) Job Description 8 years of relevant software development experience Extensive experience in C/C++ development, including a solid understanding of audio/video technologies with a commitment to delivering high-quality software through adherence to coding standards and testing practices. Must Have: Experience in C/C++, Strong in Linux system programming , good understanding what ABI is, library dependencies, cross-compilation. …</t>
+          <t>Elastic, the Search AI Company, enables everyone to find the answers they need in real time, using all their data, at scale — unleashing the potential of businesses and people. The Elastic Search AI Platform, used by more than 50% of the Fortune 500, brings together the precision of search and the intelligence of AI to enable everyone to accelerate the results that matter. By taking advantage of all structured and unstructured data — securing and protecting private information more effectively …</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1200,17 +1200,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-03-23T23:20:54Z</t>
+          <t>2025-03-23T01:05:25Z</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Senior/Staff Software Engineer - Front End Platform</t>
+          <t>Junior IT Project Manager - REMOTE WORK - 62818</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polly</t>
+          <t>PRIMUS Global Services, Inc</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1225,17 +1225,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$170,339.92 - $170,339.92</t>
+          <t>$95,274.60 - $95,274.60</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5108299538?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/land/ad/5107279675?se=GvcZky8M8BGCrnsET3cHCQ&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=C674E4EFC8BAF8F41DBDADEC791FD7EE266BA462</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Who You Are: You have 6 years of software development experience under your belt and are looking for your next challenge in a hyper-growth, fast-paced, industry disrupting, SaaS company. You are excited to work with emerging technologies and modern tech stack with a collaborative engineering team, where you will have a direct impact in the delivery of first class software products. Your experience mentoring others, working with distributed systems, relational databases, and all things software …</t>
+          <t>Job Description Job Description Junior IT Project Manager - 62818 We have an immediate long-term opportunity with one of our prime clients for the position of Junior IT Project Manager to work on Remote basis. Pay Rate : $30-$35/hr Interview Process: Initial interview with the hiring manager and other PMO Managers Second round interview with PMO Director Must Have:- Any 2-5 years IT PM who has worked on SDLC-related projects and is in Texas should work as long as communication is great. Ideal C…</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1252,22 +1252,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-03-25T07:43:28Z</t>
+          <t>2025-03-24T20:49:00Z</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>C++ Embedded Engineer</t>
+          <t>Principal Software Engineer</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>TalentOla</t>
+          <t>The Expo Group</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1277,17 +1277,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$94,271.09 - $94,271.09</t>
+          <t>$120,384.30 - $120,384.30</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014562?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5109470934?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Title: C++ Embedded Engineer Location: Dallas, TX (Onsite in office) Job Description: Experience in architecture, design, prototyping, software development, code review and unit testing for embedded devices. Experience with modern C, C++, C++11/C++14 or C++17 preferred. Experience in Embedded systems. Experience in C, C++ , embedded Linux and device driver Experience with POSIX-based embedded systems, one or more of Linux, QNX. Experience with Linux, BSP, Linux subsystems Memory and performance…</t>
+          <t>Join Our Innovative Team as a Principal Software Engineer Are you ready to drive software innovation and collaborate with a dynamic team? The Expo Group is seeking a Principal Software Engineer to design, develop, and optimize software applications that meet the needs of a growing, innovative company. Based in Irving or remotely, this role will be crucial in enhancing our software solutions while working closely with cross-functional teams to deliver scalable and efficient systems. In this role…</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1304,17 +1304,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-03-26T19:25:33Z</t>
+          <t>2025-03-24T07:57:48Z</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Technical Project Manager</t>
+          <t>ETL Developer</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Axiom Software Solutions Limited</t>
+          <t>Maximus</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1329,17 +1329,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$110,341.02 - $110,341.02</t>
+          <t>$116,170.94 - $116,170.94</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112781667?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5108715077?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Role: Technical Project Manager - Remote US Technical Project Manager with AWS, GCP experience JOB DESCRIPTION "5 years of technical program management experience in cloud infrastructure Proven track record of managing large-scale complex projects Strong technical skills and understanding of cloud computing, serverless architecture, and core infrastructure components Hands-on experience with cloud providers such as AWS, Azure, or GCP Experience in networking engineering, networking infrastructu…</t>
+          <t>Description &amp; Requirements Maximus is currently seeking a ETL Developer to work remote and join our team supporting one of our Federal clients. Essential Duties and Responsibilities: - Provide design and implementation expertise to a cross-functional software development team. - Design and develop software applications from business requirements in collaboration with other team members. - Support testing and remediate defects. - May mentor entry and mid-level developers. Project Specific Duties…</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Senior Software Engineer (BLE, C++)</t>
+          <t>C++ Developer (Audio/Video)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Highland Park</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1381,17 +1381,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>$89,213.06 - $89,213.06</t>
+          <t>$100,612.38 - $100,612.38</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014567?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5110014569?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Title: Senior Software Engineer (BLE, C++) Location: Dallas, TX (5 day onsite) Job Responsibilities Architect, develop and supervise the Linux based TV OS Bluetooth software Develop applications for smart TV Bluetooth audio and peripherals Port classic audio features of TV to LE Audio New application features using LE Audio Sustenance engineering of existing Bluetooth functionality on TV: Improvements, bug-fixes and new features Job Description 8 years of experience with C/C++, Linux/Unix and B…</t>
+          <t>Title: C++ Developer (Audio/Video) Location: Dallas, TX (5 day onsite) Job Description 8 years of relevant software development experience Extensive experience in C/C++ development, including a solid understanding of audio/video technologies with a commitment to delivering high-quality software through adherence to coding standards and testing practices. Must Have: Experience in C/C++, Strong in Linux system programming , good understanding what ABI is, library dependencies, cross-compilation. …</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1408,42 +1408,42 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-03-26T07:40:05Z</t>
+          <t>2025-03-23T01:10:57Z</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Java Full stack Developer</t>
+          <t>AVEVA/ArchestrA MES Engineer</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sumeru Solutions</t>
+          <t>Jobot</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Cockrell Hill</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>$122,468.09 - $122,468.09</t>
+          <t>$91,958.83 - $91,958.83</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5112093702?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/land/ad/5107292444?se=GvcZky8M8BGCrnsET3cHCQ&amp;utm_medium=api&amp;utm_source=08e49799&amp;v=13D6CB0DD56499F821BCA88EC93EA2288B8618F8</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Role : Java Developer Location : Dallas, TX Must Have Skills 6 years of full Software Development Life Cycle SDLC experience designing developing and implementing largescale applications in hosted production environments 2 years Microservice framework REST development Preferred Qualifications Education Prior Job Experience 2 years of Kubernetes Services with deep understanding of Container Orchestration and Distributed System Concepts Skills Licenses Certifications Proficiency in Full Stack Dev…</t>
+          <t>Controls MES Engineer - Up to $170k/yr - Free Benefits This Jobot Job is hosted by: Drew Fetter Are you a fit? Easy Apply now by clicking the "Apply Now" button and sending us your resume. Salary: $120,000 - $170,000 per year A bit about us: We are seeking an experienced Controls MES Engineer to focus on delivering business intelligence services, BI software development, and Power BI reports. Why join us? Excellent compensation package Yearly profit sharing Yearly bonus 100% free benefits 4 wee…</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1460,42 +1460,42 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-03-25T07:43:46Z</t>
+          <t>2025-03-23T23:20:54Z</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Software Engineer- Location: Addison, TX-onsite work only – Fulltime - Aerospace domain</t>
+          <t>Senior/Staff Software Engineer - Front End Platform</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Marvel Infotech</t>
+          <t>Polly</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Addison</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>$120,000.00 - $140,000.00</t>
+          <t>$170,339.92 - $170,339.92</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.adzuna.com/details/5110014904?utm_medium=api&amp;utm_source=08e49799</t>
+          <t>https://www.adzuna.com/details/5108299538?utm_medium=api&amp;utm_source=08e49799</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Software Engineer- Location: Addison, TX-onsite work only Fulltime - Aerospace domain Client needs 10 years of experience only Software Engineer This is an onsite, full-time position as part of our Engineering Team within the Software Development Group. The position is to design and implement properly documented, reliable software that ensures safe and proper execution of microprocessor and/or GUI based products/systems. Job Responsibilities Software design and development of microprocessor and…</t>
+          <t>Who You Are: You have 6 years of software development experience under your belt and are looking for your next challenge in a hyper-growth, fast-paced, industry disrupting, SaaS company. You are excited to work with emerging technologies and modern tech stack with a collaborative engineering team, where you will have a direct impact in the delivery of first class software products. Your experience mentoring others, working with distributed systems, relational databases, and all things software …</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">

</xml_diff>